<commit_message>
Atualização APIs para carga inicial dos dados
</commit_message>
<xml_diff>
--- a/AceleraPlenoProjetoFinal/AceleraPlenoProjetoFinal.Api/Resources/TIPOS_TERMINAL.xlsx
+++ b/AceleraPlenoProjetoFinal/AceleraPlenoProjetoFinal.Api/Resources/TIPOS_TERMINAL.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A523169\OneDrive - Atos\Atos_Documentos\Acelera Senior\Acelera Pleno\Trabalho conclusão de Curso\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\AceleraPlenoProjetoFinal\AceleraPlenoProjetoFinal\AceleraPlenoProjetoFinal.Api\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC61E30-061F-4A4A-8C20-70B9364E753A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122E7948-72DD-4095-9431-968EC65A30D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FD7E5DB5-0291-4B79-9A24-AC6DFF058994}"/>
+    <workbookView xWindow="-18969" yWindow="903" windowWidth="19087" windowHeight="11298" xr2:uid="{FD7E5DB5-0291-4B79-9A24-AC6DFF058994}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$E$14</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>CODIGO</t>
   </si>
@@ -88,13 +91,19 @@
   </si>
   <si>
     <t>GERENTE CORRESP. MAINOFFiCE</t>
+  </si>
+  <si>
+    <t>BOLACESSOLIBERADO</t>
+  </si>
+  <si>
+    <t>NUMCHEKALTERACAO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,8 +125,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -130,8 +147,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor theme="9" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -139,15 +174,60 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -166,9 +246,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -206,7 +286,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -312,7 +392,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -454,7 +534,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -462,20 +542,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C94A8C43-30DC-4A97-A6F5-0B2C22B2FB67}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" customWidth="1"/>
+    <col min="7" max="7" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
@@ -491,67 +571,91 @@
       <c r="E1" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2">
+        <v>8000000</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5">
+        <v>1</v>
+      </c>
+      <c r="G2" s="5">
+        <v>1802198856</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <v>10000</v>
       </c>
-      <c r="E2">
+      <c r="E3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="F3" s="6">
+        <v>0</v>
+      </c>
+      <c r="G3" s="6">
+        <v>159895520</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1">
         <v>3</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>1723468870</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1">
         <v>4</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="D4">
-        <v>40000</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5" s="1">
-        <v>5</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="D5">
         <v>40000</v>
@@ -559,161 +663,226 @@
       <c r="E5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="6">
+        <v>1</v>
+      </c>
+      <c r="G5" s="6">
+        <v>-613737432</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0</v>
       </c>
       <c r="B6" s="1">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6">
+        <v>40000</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
+        <v>544160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="B7" s="1">
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="6">
+        <v>1</v>
+      </c>
+      <c r="G7" s="6">
+        <v>-448494088</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1">
         <v>7</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>0</v>
-      </c>
-      <c r="B8" s="1">
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0</v>
+      </c>
+      <c r="G8" s="5">
+        <v>-927334048</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1">
         <v>8</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>0</v>
-      </c>
-      <c r="B9" s="1">
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0</v>
+      </c>
+      <c r="G9" s="6">
+        <v>867499134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1">
         <v>10</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="B10" s="1">
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5">
+        <v>1</v>
+      </c>
+      <c r="G10" s="5">
+        <v>-403386611</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1">
         <v>11</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D10">
+      <c r="D11">
         <v>40000</v>
       </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>0</v>
-      </c>
-      <c r="B11" s="1">
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1290899199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1">
         <v>12</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>0</v>
-      </c>
-      <c r="B12" s="1">
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0</v>
+      </c>
+      <c r="G12" s="5">
+        <v>1693967135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1">
         <v>13</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>0</v>
-      </c>
-      <c r="B13" s="1">
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0</v>
+      </c>
+      <c r="G13" s="6">
+        <v>767585788</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1">
         <v>14</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D13">
+      <c r="D14">
         <v>40000</v>
       </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>0</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14">
-        <v>8000000</v>
-      </c>
       <c r="E14">
         <v>0</v>
       </c>
+      <c r="F14" s="7">
+        <v>0</v>
+      </c>
+      <c r="G14" s="7">
+        <v>2107579721</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E14" xr:uid="{C94A8C43-30DC-4A97-A6F5-0B2C22B2FB67}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E14">
+      <sortCondition ref="B1:B14"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>